<commit_message>
Updated Files before Grant Left
</commit_message>
<xml_diff>
--- a/IT3-Schedule.xlsx
+++ b/IT3-Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/jsp69_pitt_edu/Documents/Engineering/ECE 1140/System/ECE-1140-Group-5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zkubi\OneDrive\Documents\ECE1140\Python Code\New Project\ECE-1140-Group-5-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{897584AF-B201-44A1-B6A1-E2790C02790F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F7B88E99-7BBB-4040-A360-FA625ADE2573}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED71905-053E-4818-8051-9B80E931B883}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FA2CB412-298D-E148-AF01-A7BF1C50A06E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA2CB412-298D-E148-AF01-A7BF1C50A06E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Line</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>UNDER</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
   </si>
 </sst>
 </file>
@@ -600,39 +606,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCED271-4E5B-8C49-8383-277E47755BB7}">
-  <dimension ref="A1:AQ163"/>
+  <dimension ref="A1:AQ162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="12"/>
-    <col min="2" max="2" width="12.875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.8984375" style="12"/>
+    <col min="2" max="2" width="12.8984375" style="12" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="23.125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="30.875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="23.09765625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="30.8984375" style="12" customWidth="1"/>
     <col min="6" max="6" width="43" style="12" customWidth="1"/>
-    <col min="7" max="7" width="35.875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="35.8984375" style="12" customWidth="1"/>
     <col min="8" max="12" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="8.875" style="3" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="8.8984375" style="3" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="4.5" style="3" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="3.5" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="23" width="8.875" style="3" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="19.375" style="3" hidden="1" customWidth="1"/>
+    <col min="20" max="23" width="8.8984375" style="3" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="19.3984375" style="3" hidden="1" customWidth="1"/>
     <col min="25" max="28" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="11.875" style="3" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="11.8984375" style="3" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="25.375" style="3" customWidth="1"/>
-    <col min="32" max="36" width="10.625" style="22" customWidth="1"/>
-    <col min="37" max="41" width="8.875" style="12"/>
+    <col min="31" max="31" width="25.3984375" style="3" customWidth="1"/>
+    <col min="32" max="36" width="10.59765625" style="22" customWidth="1"/>
+    <col min="37" max="41" width="8.8984375" style="12"/>
     <col min="42" max="42" width="4.5" style="3" customWidth="1"/>
-    <col min="43" max="16384" width="8.875" style="3"/>
+    <col min="43" max="16384" width="8.8984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +738,7 @@
       <c r="AO1" s="10"/>
       <c r="AQ1" s="11"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>28</v>
       </c>
@@ -772,9 +778,9 @@
         <f>L2-(M2*$AA$2)</f>
         <v>-34.467676767676771</v>
       </c>
-      <c r="Z2" s="14">
-        <f t="shared" ref="Z2:Z14" si="0">L2-(M2+M3)*$AA$2</f>
-        <v>-73.553391053391067</v>
+      <c r="Z2" s="14" t="e">
+        <f>L2-(M2+#REF!)*$AA$2</f>
+        <v>#REF!</v>
       </c>
       <c r="AA2" s="15">
         <v>7.6</v>
@@ -792,7 +798,7 @@
       <c r="AN2" s="16"/>
       <c r="AO2" s="16"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>28</v>
       </c>
@@ -811,98 +817,47 @@
       <c r="F3" s="12">
         <v>70</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="12" t="s">
         <v>33</v>
       </c>
       <c r="I3" s="12">
-        <f t="shared" ref="I3:I14" si="1">E3*D3/100</f>
+        <f t="shared" ref="I3:I13" si="0">E3*D3/100</f>
         <v>0</v>
       </c>
-      <c r="J3" s="12">
-        <f>I3+J2</f>
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="12"/>
+      <c r="J3" s="12" t="e">
+        <f>I3+#REF!</f>
+        <v>#REF!</v>
+      </c>
       <c r="L3" s="13">
-        <f t="shared" ref="L3:L14" si="2">F3*1000/60/60</f>
+        <f t="shared" ref="L3:L13" si="1">F3*1000/60/60</f>
         <v>19.444444444444446</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M14" si="3">D3/L3</f>
+        <f t="shared" ref="M3:M13" si="2">D3/L3</f>
         <v>5.1428571428571423</v>
       </c>
-      <c r="N3" s="18">
-        <f>SUM(M2:M3)+SUM(M5:M9)</f>
-        <v>55.402597402597394</v>
-      </c>
-      <c r="O3" s="13">
-        <f>L3/$R$1</f>
-        <v>38.888888888888893</v>
-      </c>
-      <c r="P3" s="13">
-        <f>0.5*$R$1*O3*O3</f>
-        <v>378.08641975308649</v>
-      </c>
-      <c r="Q3" s="3">
-        <f>SUM(D2:D3)+SUM(D5:D9)</f>
-        <v>900</v>
-      </c>
-      <c r="T3" s="13">
-        <f>2*O3</f>
-        <v>77.777777777777786</v>
-      </c>
-      <c r="U3" s="13">
-        <f>(Q3-2*P3)/L3</f>
-        <v>7.3968253968253892</v>
-      </c>
-      <c r="V3" s="18">
-        <f>U3+T3</f>
-        <v>85.174603174603178</v>
-      </c>
-      <c r="W3" s="3">
-        <v>60</v>
-      </c>
-      <c r="X3" s="14">
-        <f>(V3+W3)/60</f>
-        <v>2.4195767195767197</v>
-      </c>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
       <c r="Y3" s="14">
-        <f t="shared" ref="Y3:Y14" si="4">L3-(M3*$AA$2)</f>
+        <f t="shared" ref="Y3:Y13" si="3">L3-(M3*$AA$2)</f>
         <v>-19.641269841269835</v>
       </c>
       <c r="Z3" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Z3:Z13" si="4">L3-(M3+M4)*$AA$2</f>
         <v>-58.726984126984121</v>
       </c>
-      <c r="AB3" s="18">
-        <f>SUM(M2:M3)</f>
-        <v>11.688311688311689</v>
-      </c>
-      <c r="AC3" s="18">
-        <f>AB3*2</f>
-        <v>23.376623376623378</v>
-      </c>
-      <c r="AD3" s="18">
-        <f>AC3</f>
-        <v>23.376623376623378</v>
-      </c>
-      <c r="AE3" s="19">
+      <c r="AE3" s="3">
         <v>0</v>
       </c>
       <c r="AF3" s="16">
         <v>0.11944444444444445</v>
       </c>
-      <c r="AG3" s="16"/>
-      <c r="AH3" s="16"/>
-      <c r="AI3" s="16"/>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="16"/>
-      <c r="AL3" s="16"/>
-      <c r="AM3" s="16"/>
-      <c r="AN3" s="16"/>
-      <c r="AO3" s="16"/>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>28</v>
       </c>
@@ -910,7 +865,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="12">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" s="12">
         <v>100</v>
@@ -922,30 +877,30 @@
         <v>70</v>
       </c>
       <c r="I4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="12" t="e">
+        <f t="shared" ref="J4:J13" si="5">I4+J3</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L4" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="12">
-        <f t="shared" ref="J4:J14" si="5">I4+J3</f>
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="13">
+        <v>19.444444444444446</v>
+      </c>
+      <c r="M4" s="13">
         <f t="shared" si="2"/>
-        <v>19.444444444444446</v>
-      </c>
-      <c r="M4" s="13">
-        <f t="shared" si="3"/>
         <v>5.1428571428571423</v>
       </c>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Y4" s="14">
+        <f t="shared" si="3"/>
+        <v>-19.641269841269835</v>
+      </c>
+      <c r="Z4" s="14">
         <f t="shared" si="4"/>
-        <v>-19.641269841269835</v>
-      </c>
-      <c r="Z4" s="14">
-        <f t="shared" si="0"/>
-        <v>-58.726984126984121</v>
+        <v>-97.812698412698396</v>
       </c>
       <c r="AF4" s="12"/>
       <c r="AG4" s="12"/>
@@ -953,18 +908,18 @@
       <c r="AI4" s="12"/>
       <c r="AJ4" s="12"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="12">
-        <v>64</v>
+      <c r="C5" s="13">
+        <v>65</v>
       </c>
       <c r="D5" s="12">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
@@ -972,47 +927,48 @@
       <c r="F5" s="12">
         <v>70</v>
       </c>
+      <c r="G5" s="17"/>
       <c r="I5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L5" s="13">
+        <v>19.444444444444446</v>
+      </c>
+      <c r="M5" s="13">
         <f t="shared" si="2"/>
-        <v>19.444444444444446</v>
-      </c>
-      <c r="M5" s="13">
-        <f t="shared" si="3"/>
-        <v>5.1428571428571423</v>
+        <v>10.285714285714285</v>
       </c>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
       <c r="Y5" s="14">
+        <f t="shared" si="3"/>
+        <v>-58.726984126984121</v>
+      </c>
+      <c r="Z5" s="14">
         <f t="shared" si="4"/>
-        <v>-19.641269841269835</v>
-      </c>
-      <c r="Z5" s="14">
-        <f t="shared" si="0"/>
-        <v>-97.812698412698396</v>
-      </c>
-      <c r="AF5" s="12"/>
+        <v>-136.89841269841267</v>
+      </c>
+      <c r="AF5" s="16"/>
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="12"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="13">
-        <v>65</v>
+      <c r="C6" s="12">
+        <v>66</v>
       </c>
       <c r="D6" s="12">
         <v>200</v>
@@ -1023,40 +979,39 @@
       <c r="F6" s="12">
         <v>70</v>
       </c>
-      <c r="G6" s="17"/>
       <c r="I6" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L6" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L6" s="13">
+        <v>19.444444444444446</v>
+      </c>
+      <c r="M6" s="13">
         <f t="shared" si="2"/>
-        <v>19.444444444444446</v>
-      </c>
-      <c r="M6" s="13">
-        <f t="shared" si="3"/>
         <v>10.285714285714285</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Y6" s="14">
+        <f t="shared" si="3"/>
+        <v>-58.726984126984121</v>
+      </c>
+      <c r="Z6" s="14">
         <f t="shared" si="4"/>
-        <v>-58.726984126984121</v>
-      </c>
-      <c r="Z6" s="14">
-        <f t="shared" si="0"/>
-        <v>-136.89841269841267</v>
-      </c>
-      <c r="AF6" s="16"/>
+        <v>-127.12698412698411</v>
+      </c>
+      <c r="AF6" s="12"/>
       <c r="AG6" s="12"/>
       <c r="AH6" s="12"/>
       <c r="AI6" s="12"/>
       <c r="AJ6" s="12"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>28</v>
       </c>
@@ -1064,42 +1019,43 @@
         <v>29</v>
       </c>
       <c r="C7" s="12">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7" s="12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
       </c>
       <c r="F7" s="12">
-        <v>70</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G7" s="17"/>
       <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L7" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M7" s="13">
         <f t="shared" si="2"/>
-        <v>19.444444444444446</v>
-      </c>
-      <c r="M7" s="13">
-        <f t="shared" si="3"/>
-        <v>10.285714285714285</v>
+        <v>9</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Y7" s="14">
+        <f t="shared" si="3"/>
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z7" s="14">
         <f t="shared" si="4"/>
-        <v>-58.726984126984121</v>
-      </c>
-      <c r="Z7" s="14">
-        <f t="shared" si="0"/>
-        <v>-127.12698412698411</v>
+        <v>-125.68888888888887</v>
       </c>
       <c r="AF7" s="12"/>
       <c r="AG7" s="12"/>
@@ -1107,15 +1063,15 @@
       <c r="AI7" s="12"/>
       <c r="AJ7" s="12"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="12">
-        <v>67</v>
+      <c r="C8" s="13">
+        <v>68</v>
       </c>
       <c r="D8" s="12">
         <v>100</v>
@@ -1126,31 +1082,30 @@
       <c r="F8" s="12">
         <v>40</v>
       </c>
-      <c r="G8" s="17"/>
       <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L8" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M8" s="13">
         <f t="shared" si="2"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="M8" s="13">
-        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Y8" s="14">
+        <f t="shared" si="3"/>
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z8" s="14">
         <f t="shared" si="4"/>
-        <v>-57.288888888888877</v>
-      </c>
-      <c r="Z8" s="14">
-        <f t="shared" si="0"/>
         <v>-125.68888888888887</v>
       </c>
       <c r="AF8" s="12"/>
@@ -1159,15 +1114,15 @@
       <c r="AI8" s="12"/>
       <c r="AJ8" s="12"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="13">
-        <v>68</v>
+        <v>30</v>
+      </c>
+      <c r="C9" s="12">
+        <v>69</v>
       </c>
       <c r="D9" s="12">
         <v>100</v>
@@ -1178,39 +1133,91 @@
       <c r="F9" s="12">
         <v>40</v>
       </c>
+      <c r="G9" s="17"/>
       <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M9" s="13">
         <f t="shared" si="2"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="M9" s="13">
+        <v>9</v>
+      </c>
+      <c r="N9" s="18">
+        <f>SUM(M3:M9)</f>
+        <v>57.857142857142854</v>
+      </c>
+      <c r="O9" s="13">
+        <f>L9/$R$1</f>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="P9" s="13">
+        <f t="shared" ref="P9" si="6">0.5*$R$1*O9*O9</f>
+        <v>123.45679012345678</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>SUM(D3:D9)</f>
+        <v>900</v>
+      </c>
+      <c r="T9" s="13">
+        <f>2*O9</f>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="U9" s="13">
+        <f>(Q9-2*P9)/L9</f>
+        <v>58.777777777777779</v>
+      </c>
+      <c r="V9" s="18">
+        <f>U9+T9</f>
+        <v>103.22222222222223</v>
+      </c>
+      <c r="W9" s="3">
+        <v>60</v>
+      </c>
+      <c r="X9" s="14">
+        <f>(V9+W9)/60</f>
+        <v>2.7203703703703703</v>
+      </c>
+      <c r="Y9" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Y9" s="14">
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z9" s="14">
         <f t="shared" si="4"/>
-        <v>-57.288888888888877</v>
-      </c>
-      <c r="Z9" s="14">
-        <f t="shared" si="0"/>
         <v>-125.68888888888887</v>
       </c>
-      <c r="AF9" s="12"/>
-      <c r="AG9" s="12"/>
-      <c r="AH9" s="12"/>
-      <c r="AI9" s="12"/>
-      <c r="AJ9" s="12"/>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AB9" s="18">
+        <f>SUM(M3:M9)</f>
+        <v>57.857142857142854</v>
+      </c>
+      <c r="AC9" s="18">
+        <f>AB9*2+120</f>
+        <v>235.71428571428572</v>
+      </c>
+      <c r="AD9" s="18" t="e">
+        <f>AC9+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AE9" s="19"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="16"/>
+      <c r="AN9" s="16"/>
+      <c r="AO9" s="16"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>28</v>
       </c>
@@ -1218,7 +1225,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="12">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D10" s="12">
         <v>100</v>
@@ -1229,99 +1236,45 @@
       <c r="F10" s="12">
         <v>40</v>
       </c>
-      <c r="G10" s="17"/>
       <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L10" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M10" s="13">
         <f t="shared" si="2"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="M10" s="13">
+        <v>9</v>
+      </c>
+      <c r="Y10" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="N10" s="18">
-        <f>SUM(M4:M10)</f>
-        <v>57.857142857142854</v>
-      </c>
-      <c r="O10" s="13">
-        <f>L10/$R$1</f>
-        <v>22.222222222222221</v>
-      </c>
-      <c r="P10" s="13">
-        <f t="shared" ref="P10" si="6">0.5*$R$1*O10*O10</f>
-        <v>123.45679012345678</v>
-      </c>
-      <c r="Q10" s="3">
-        <f>SUM(D4:D10)</f>
-        <v>900</v>
-      </c>
-      <c r="T10" s="13">
-        <f>2*O10</f>
-        <v>44.444444444444443</v>
-      </c>
-      <c r="U10" s="13">
-        <f>(Q10-2*P10)/L10</f>
-        <v>58.777777777777779</v>
-      </c>
-      <c r="V10" s="18">
-        <f>U10+T10</f>
-        <v>103.22222222222223</v>
-      </c>
-      <c r="W10" s="3">
-        <v>60</v>
-      </c>
-      <c r="X10" s="14">
-        <f>(V10+W10)/60</f>
-        <v>2.7203703703703703</v>
-      </c>
-      <c r="Y10" s="14">
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z10" s="14">
         <f t="shared" si="4"/>
-        <v>-57.288888888888877</v>
-      </c>
-      <c r="Z10" s="14">
-        <f t="shared" si="0"/>
         <v>-125.68888888888887</v>
       </c>
-      <c r="AB10" s="18">
-        <f>SUM(M4:M10)</f>
-        <v>57.857142857142854</v>
-      </c>
-      <c r="AC10" s="18">
-        <f>AB10*2+120</f>
-        <v>235.71428571428572</v>
-      </c>
-      <c r="AD10" s="18">
-        <f>AC10+AD3</f>
-        <v>259.09090909090912</v>
-      </c>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="16"/>
-      <c r="AG10" s="16"/>
-      <c r="AH10" s="16"/>
-      <c r="AI10" s="16"/>
-      <c r="AJ10" s="16"/>
-      <c r="AK10" s="16"/>
-      <c r="AL10" s="16"/>
-      <c r="AM10" s="16"/>
-      <c r="AN10" s="16"/>
-      <c r="AO10" s="16"/>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="12">
-        <v>70</v>
+      <c r="C11" s="13">
+        <v>71</v>
       </c>
       <c r="D11" s="12">
         <v>100</v>
@@ -1333,27 +1286,27 @@
         <v>40</v>
       </c>
       <c r="I11" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L11" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M11" s="13">
         <f t="shared" si="2"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="M11" s="13">
+        <v>9</v>
+      </c>
+      <c r="Y11" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="Y11" s="14">
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z11" s="14">
         <f t="shared" si="4"/>
-        <v>-57.288888888888877</v>
-      </c>
-      <c r="Z11" s="14">
-        <f t="shared" si="0"/>
         <v>-125.68888888888887</v>
       </c>
       <c r="AF11" s="12"/>
@@ -1362,15 +1315,15 @@
       <c r="AI11" s="12"/>
       <c r="AJ11" s="12"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="13">
-        <v>71</v>
+      <c r="C12" s="12">
+        <v>72</v>
       </c>
       <c r="D12" s="12">
         <v>100</v>
@@ -1382,27 +1335,27 @@
         <v>40</v>
       </c>
       <c r="I12" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L12" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L12" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M12" s="13">
         <f t="shared" si="2"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="M12" s="13">
+        <v>9</v>
+      </c>
+      <c r="Y12" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="Y12" s="14">
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z12" s="14">
         <f t="shared" si="4"/>
-        <v>-57.288888888888877</v>
-      </c>
-      <c r="Z12" s="14">
-        <f t="shared" si="0"/>
         <v>-125.68888888888887</v>
       </c>
       <c r="AF12" s="12"/>
@@ -1411,7 +1364,7 @@
       <c r="AI12" s="12"/>
       <c r="AJ12" s="12"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1372,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="12">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D13" s="12">
         <v>100</v>
@@ -1430,45 +1383,46 @@
       <c r="F13" s="12">
         <v>40</v>
       </c>
+      <c r="G13" s="17"/>
       <c r="I13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="L13" s="13">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M13" s="13">
         <f t="shared" si="2"/>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="M13" s="13">
+        <v>9</v>
+      </c>
+      <c r="Y13" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="Y13" s="14">
+        <v>-57.288888888888877</v>
+      </c>
+      <c r="Z13" s="14">
         <f t="shared" si="4"/>
-        <v>-57.288888888888877</v>
-      </c>
-      <c r="Z13" s="14">
-        <f t="shared" si="0"/>
         <v>-125.68888888888887</v>
       </c>
-      <c r="AF13" s="12"/>
+      <c r="AF13" s="16"/>
       <c r="AG13" s="12"/>
       <c r="AH13" s="12"/>
       <c r="AI13" s="12"/>
       <c r="AJ13" s="12"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C14" s="12">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="12">
         <v>100</v>
@@ -1479,45 +1433,56 @@
       <c r="F14" s="12">
         <v>40</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>31</v>
-      </c>
+      <c r="G14" s="17"/>
       <c r="I14" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I14" si="7">E14*D14/100</f>
         <v>0</v>
       </c>
-      <c r="J14" s="12">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
+      <c r="J14" s="12" t="e">
+        <f t="shared" ref="J14" si="8">I14+J13</f>
+        <v>#REF!</v>
       </c>
       <c r="L14" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L14" si="9">F14*1000/60/60</f>
         <v>11.111111111111111</v>
       </c>
       <c r="M14" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="M14" si="10">D14/L14</f>
         <v>9</v>
       </c>
       <c r="Y14" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="Y14" si="11">L14-(M14*$AA$2)</f>
         <v>-57.288888888888877</v>
       </c>
       <c r="Z14" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Z14" si="12">L14-(M14+M15)*$AA$2</f>
         <v>-57.288888888888877</v>
       </c>
-      <c r="AE14" s="3">
-        <v>8</v>
-      </c>
-      <c r="AF14" s="16">
-        <v>0.125</v>
-      </c>
+      <c r="AF14" s="16"/>
       <c r="AG14" s="12"/>
       <c r="AH14" s="12"/>
       <c r="AI14" s="12"/>
       <c r="AJ14" s="12"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="12">
+        <v>75</v>
+      </c>
+      <c r="D15" s="12">
+        <v>100</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0</v>
+      </c>
+      <c r="F15" s="12">
+        <v>40</v>
+      </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="L15" s="13"/>
@@ -1530,52 +1495,96 @@
       <c r="AI15" s="12"/>
       <c r="AJ15" s="12"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="C16" s="13"/>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="12">
+        <v>76</v>
+      </c>
+      <c r="D16" s="12">
+        <v>100</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
+        <v>40</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="18"/>
+      <c r="X16" s="14"/>
       <c r="Y16" s="14"/>
       <c r="Z16" s="14"/>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="12"/>
-      <c r="AI16" s="12"/>
-      <c r="AJ16" s="12"/>
-    </row>
-    <row r="17" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G17" s="17"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="19"/>
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="16"/>
+      <c r="AI16" s="16"/>
+      <c r="AJ16" s="16"/>
+      <c r="AK16" s="16"/>
+      <c r="AL16" s="16"/>
+      <c r="AM16" s="16"/>
+      <c r="AN16" s="16"/>
+      <c r="AO16" s="16"/>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="12">
+        <v>77</v>
+      </c>
+      <c r="D17" s="12">
+        <v>100</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>40</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>31</v>
+      </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="18"/>
-      <c r="X17" s="14"/>
       <c r="Y17" s="14"/>
       <c r="Z17" s="14"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="19"/>
-      <c r="AF17" s="16"/>
-      <c r="AG17" s="16"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
-      <c r="AJ17" s="16"/>
-      <c r="AK17" s="16"/>
-      <c r="AL17" s="16"/>
-      <c r="AM17" s="16"/>
-      <c r="AN17" s="16"/>
-      <c r="AO17" s="16"/>
-    </row>
-    <row r="18" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
+      <c r="AE17" s="3">
+        <v>8</v>
+      </c>
+      <c r="AF17" s="16">
+        <v>0.125</v>
+      </c>
+      <c r="AG17" s="12"/>
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="12"/>
+      <c r="AJ17" s="12"/>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="L18" s="13"/>
@@ -1588,7 +1597,7 @@
       <c r="AI18" s="12"/>
       <c r="AJ18" s="12"/>
     </row>
-    <row r="19" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="L19" s="13"/>
@@ -1601,7 +1610,8 @@
       <c r="AI19" s="12"/>
       <c r="AJ19" s="12"/>
     </row>
-    <row r="20" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="C20" s="13"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="L20" s="13"/>
@@ -1614,8 +1624,7 @@
       <c r="AI20" s="12"/>
       <c r="AJ20" s="12"/>
     </row>
-    <row r="21" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C21" s="13"/>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="L21" s="13"/>
@@ -1628,51 +1637,51 @@
       <c r="AI21" s="12"/>
       <c r="AJ21" s="12"/>
     </row>
-    <row r="22" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="C22" s="13"/>
+      <c r="G22" s="17"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="18"/>
+      <c r="X22" s="14"/>
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
-      <c r="AF22" s="12"/>
-      <c r="AG22" s="12"/>
-      <c r="AH22" s="12"/>
-      <c r="AI22" s="12"/>
-      <c r="AJ22" s="12"/>
-    </row>
-    <row r="23" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-      <c r="G23" s="17"/>
+      <c r="AB22" s="18"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="18"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="16"/>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="16"/>
+      <c r="AI22" s="16"/>
+      <c r="AJ22" s="16"/>
+      <c r="AK22" s="16"/>
+      <c r="AL22" s="16"/>
+      <c r="AM22" s="16"/>
+      <c r="AN22" s="16"/>
+      <c r="AO22" s="16"/>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="18"/>
-      <c r="X23" s="14"/>
       <c r="Y23" s="14"/>
       <c r="Z23" s="14"/>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="18"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="16"/>
-      <c r="AH23" s="16"/>
-      <c r="AI23" s="16"/>
-      <c r="AJ23" s="16"/>
-      <c r="AK23" s="16"/>
-      <c r="AL23" s="16"/>
-      <c r="AM23" s="16"/>
-      <c r="AN23" s="16"/>
-      <c r="AO23" s="16"/>
-    </row>
-    <row r="24" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+      <c r="AH23" s="12"/>
+      <c r="AI23" s="12"/>
+      <c r="AJ23" s="12"/>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="L24" s="13"/>
@@ -1685,7 +1694,8 @@
       <c r="AI24" s="12"/>
       <c r="AJ24" s="12"/>
     </row>
-    <row r="25" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="C25" s="13"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="L25" s="13"/>
@@ -1698,8 +1708,7 @@
       <c r="AI25" s="12"/>
       <c r="AJ25" s="12"/>
     </row>
-    <row r="26" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C26" s="13"/>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="L26" s="13"/>
@@ -1712,7 +1721,8 @@
       <c r="AI26" s="12"/>
       <c r="AJ26" s="12"/>
     </row>
-    <row r="27" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="C27" s="13"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="L27" s="13"/>
@@ -1725,8 +1735,7 @@
       <c r="AI27" s="12"/>
       <c r="AJ27" s="12"/>
     </row>
-    <row r="28" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C28" s="13"/>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="L28" s="13"/>
@@ -1739,7 +1748,7 @@
       <c r="AI28" s="12"/>
       <c r="AJ28" s="12"/>
     </row>
-    <row r="29" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="L29" s="13"/>
@@ -1752,7 +1761,8 @@
       <c r="AI29" s="12"/>
       <c r="AJ29" s="12"/>
     </row>
-    <row r="30" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="C30" s="13"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="L30" s="13"/>
@@ -1765,52 +1775,51 @@
       <c r="AI30" s="12"/>
       <c r="AJ30" s="12"/>
     </row>
-    <row r="31" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C31" s="13"/>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="G31" s="17"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="18"/>
+      <c r="X31" s="14"/>
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
-      <c r="AF31" s="12"/>
-      <c r="AG31" s="12"/>
-      <c r="AH31" s="12"/>
-      <c r="AI31" s="12"/>
-      <c r="AJ31" s="12"/>
-    </row>
-    <row r="32" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G32" s="17"/>
+      <c r="AB31" s="18"/>
+      <c r="AC31" s="18"/>
+      <c r="AD31" s="18"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="16"/>
+      <c r="AG31" s="16"/>
+      <c r="AH31" s="16"/>
+      <c r="AI31" s="16"/>
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="16"/>
+      <c r="AL31" s="16"/>
+      <c r="AM31" s="16"/>
+      <c r="AN31" s="16"/>
+      <c r="AO31" s="16"/>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="C32" s="13"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="T32" s="13"/>
-      <c r="U32" s="13"/>
-      <c r="V32" s="18"/>
-      <c r="X32" s="14"/>
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="19"/>
-      <c r="AF32" s="16"/>
-      <c r="AG32" s="16"/>
-      <c r="AH32" s="16"/>
-      <c r="AI32" s="16"/>
-      <c r="AJ32" s="16"/>
-      <c r="AK32" s="16"/>
-      <c r="AL32" s="16"/>
-      <c r="AM32" s="16"/>
-      <c r="AN32" s="16"/>
-      <c r="AO32" s="16"/>
-    </row>
-    <row r="33" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C33" s="13"/>
+      <c r="AF32" s="12"/>
+      <c r="AG32" s="12"/>
+      <c r="AH32" s="12"/>
+      <c r="AI32" s="12"/>
+      <c r="AJ32" s="12"/>
+    </row>
+    <row r="33" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="L33" s="13"/>
@@ -1823,7 +1832,7 @@
       <c r="AI33" s="12"/>
       <c r="AJ33" s="12"/>
     </row>
-    <row r="34" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="L34" s="13"/>
@@ -1836,7 +1845,8 @@
       <c r="AI34" s="12"/>
       <c r="AJ34" s="12"/>
     </row>
-    <row r="35" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C35" s="13"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="L35" s="13"/>
@@ -1849,8 +1859,7 @@
       <c r="AI35" s="12"/>
       <c r="AJ35" s="12"/>
     </row>
-    <row r="36" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C36" s="13"/>
+    <row r="36" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="L36" s="13"/>
@@ -1863,7 +1872,7 @@
       <c r="AI36" s="12"/>
       <c r="AJ36" s="12"/>
     </row>
-    <row r="37" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="L37" s="13"/>
@@ -1876,7 +1885,8 @@
       <c r="AI37" s="12"/>
       <c r="AJ37" s="12"/>
     </row>
-    <row r="38" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C38" s="13"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
       <c r="L38" s="13"/>
@@ -1889,51 +1899,51 @@
       <c r="AI38" s="12"/>
       <c r="AJ38" s="12"/>
     </row>
-    <row r="39" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C39" s="13"/>
+    <row r="39" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G39" s="17"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="18"/>
+      <c r="X39" s="14"/>
       <c r="Y39" s="14"/>
       <c r="Z39" s="14"/>
-      <c r="AF39" s="12"/>
-      <c r="AG39" s="12"/>
-      <c r="AH39" s="12"/>
-      <c r="AI39" s="12"/>
-      <c r="AJ39" s="12"/>
-    </row>
-    <row r="40" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G40" s="17"/>
+      <c r="AB39" s="18"/>
+      <c r="AC39" s="18"/>
+      <c r="AD39" s="18"/>
+      <c r="AE39" s="19"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="16"/>
+      <c r="AI39" s="16"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="16"/>
+      <c r="AL39" s="16"/>
+      <c r="AM39" s="16"/>
+      <c r="AN39" s="16"/>
+      <c r="AO39" s="16"/>
+    </row>
+    <row r="40" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
       <c r="L40" s="13"/>
       <c r="M40" s="13"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="13"/>
-      <c r="T40" s="13"/>
-      <c r="U40" s="13"/>
-      <c r="V40" s="18"/>
-      <c r="X40" s="14"/>
       <c r="Y40" s="14"/>
       <c r="Z40" s="14"/>
-      <c r="AB40" s="18"/>
-      <c r="AC40" s="18"/>
-      <c r="AD40" s="18"/>
-      <c r="AE40" s="19"/>
-      <c r="AF40" s="16"/>
-      <c r="AG40" s="16"/>
-      <c r="AH40" s="16"/>
-      <c r="AI40" s="16"/>
-      <c r="AJ40" s="16"/>
-      <c r="AK40" s="16"/>
-      <c r="AL40" s="16"/>
-      <c r="AM40" s="16"/>
-      <c r="AN40" s="16"/>
-      <c r="AO40" s="16"/>
-    </row>
-    <row r="41" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+      <c r="AH40" s="12"/>
+      <c r="AI40" s="12"/>
+      <c r="AJ40" s="12"/>
+    </row>
+    <row r="41" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C41" s="13"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="L41" s="13"/>
@@ -1946,8 +1956,7 @@
       <c r="AI41" s="12"/>
       <c r="AJ41" s="12"/>
     </row>
-    <row r="42" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C42" s="13"/>
+    <row r="42" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="L42" s="13"/>
@@ -1960,7 +1969,7 @@
       <c r="AI42" s="12"/>
       <c r="AJ42" s="12"/>
     </row>
-    <row r="43" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
       <c r="L43" s="13"/>
@@ -1973,7 +1982,8 @@
       <c r="AI43" s="12"/>
       <c r="AJ43" s="12"/>
     </row>
-    <row r="44" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C44" s="13"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="L44" s="13"/>
@@ -1986,8 +1996,7 @@
       <c r="AI44" s="12"/>
       <c r="AJ44" s="12"/>
     </row>
-    <row r="45" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C45" s="13"/>
+    <row r="45" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="L45" s="13"/>
@@ -2000,7 +2009,7 @@
       <c r="AI45" s="12"/>
       <c r="AJ45" s="12"/>
     </row>
-    <row r="46" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
       <c r="L46" s="13"/>
@@ -2013,7 +2022,8 @@
       <c r="AI46" s="12"/>
       <c r="AJ46" s="12"/>
     </row>
-    <row r="47" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C47" s="13"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
       <c r="L47" s="13"/>
@@ -2026,51 +2036,51 @@
       <c r="AI47" s="12"/>
       <c r="AJ47" s="12"/>
     </row>
-    <row r="48" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C48" s="13"/>
+    <row r="48" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G48" s="17"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="18"/>
+      <c r="X48" s="14"/>
       <c r="Y48" s="14"/>
       <c r="Z48" s="14"/>
-      <c r="AF48" s="12"/>
-      <c r="AG48" s="12"/>
-      <c r="AH48" s="12"/>
-      <c r="AI48" s="12"/>
-      <c r="AJ48" s="12"/>
-    </row>
-    <row r="49" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G49" s="17"/>
+      <c r="AB48" s="18"/>
+      <c r="AC48" s="18"/>
+      <c r="AD48" s="18"/>
+      <c r="AE48" s="19"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+      <c r="AI48" s="16"/>
+      <c r="AJ48" s="16"/>
+      <c r="AK48" s="16"/>
+      <c r="AL48" s="16"/>
+      <c r="AM48" s="16"/>
+      <c r="AN48" s="16"/>
+      <c r="AO48" s="16"/>
+    </row>
+    <row r="49" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="L49" s="13"/>
       <c r="M49" s="13"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="20"/>
-      <c r="P49" s="13"/>
-      <c r="T49" s="13"/>
-      <c r="U49" s="13"/>
-      <c r="V49" s="18"/>
-      <c r="X49" s="14"/>
       <c r="Y49" s="14"/>
       <c r="Z49" s="14"/>
-      <c r="AB49" s="18"/>
-      <c r="AC49" s="18"/>
-      <c r="AD49" s="18"/>
-      <c r="AE49" s="19"/>
-      <c r="AF49" s="16"/>
-      <c r="AG49" s="16"/>
-      <c r="AH49" s="16"/>
-      <c r="AI49" s="16"/>
-      <c r="AJ49" s="16"/>
-      <c r="AK49" s="16"/>
-      <c r="AL49" s="16"/>
-      <c r="AM49" s="16"/>
-      <c r="AN49" s="16"/>
-      <c r="AO49" s="16"/>
-    </row>
-    <row r="50" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AF49" s="12"/>
+      <c r="AG49" s="12"/>
+      <c r="AH49" s="12"/>
+      <c r="AI49" s="12"/>
+      <c r="AJ49" s="12"/>
+    </row>
+    <row r="50" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C50" s="13"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
       <c r="L50" s="13"/>
@@ -2083,8 +2093,7 @@
       <c r="AI50" s="12"/>
       <c r="AJ50" s="12"/>
     </row>
-    <row r="51" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C51" s="13"/>
+    <row r="51" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
       <c r="L51" s="13"/>
@@ -2097,7 +2106,7 @@
       <c r="AI51" s="12"/>
       <c r="AJ51" s="12"/>
     </row>
-    <row r="52" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
       <c r="L52" s="13"/>
@@ -2110,7 +2119,8 @@
       <c r="AI52" s="12"/>
       <c r="AJ52" s="12"/>
     </row>
-    <row r="53" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C53" s="13"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="L53" s="13"/>
@@ -2123,8 +2133,7 @@
       <c r="AI53" s="12"/>
       <c r="AJ53" s="12"/>
     </row>
-    <row r="54" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C54" s="13"/>
+    <row r="54" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
       <c r="L54" s="13"/>
@@ -2137,7 +2146,7 @@
       <c r="AI54" s="12"/>
       <c r="AJ54" s="12"/>
     </row>
-    <row r="55" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
       <c r="L55" s="13"/>
@@ -2150,7 +2159,8 @@
       <c r="AI55" s="12"/>
       <c r="AJ55" s="12"/>
     </row>
-    <row r="56" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C56" s="13"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
       <c r="L56" s="13"/>
@@ -2163,52 +2173,52 @@
       <c r="AI56" s="12"/>
       <c r="AJ56" s="12"/>
     </row>
-    <row r="57" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C57" s="13"/>
+    <row r="57" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G57" s="17"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
       <c r="L57" s="13"/>
       <c r="M57" s="13"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="13"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="18"/>
+      <c r="X57" s="14"/>
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
-      <c r="AF57" s="12"/>
-      <c r="AG57" s="12"/>
-      <c r="AH57" s="12"/>
-      <c r="AI57" s="12"/>
-      <c r="AJ57" s="12"/>
-    </row>
-    <row r="58" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AB57" s="18"/>
+      <c r="AC57" s="18"/>
+      <c r="AD57" s="18"/>
+      <c r="AE57" s="19"/>
+      <c r="AF57" s="16"/>
+      <c r="AG57" s="16"/>
+      <c r="AH57" s="16"/>
+      <c r="AI57" s="16"/>
+      <c r="AJ57" s="16"/>
+      <c r="AK57" s="16"/>
+      <c r="AL57" s="16"/>
+      <c r="AM57" s="16"/>
+      <c r="AN57" s="16"/>
+      <c r="AO57" s="16"/>
+    </row>
+    <row r="58" spans="3:41" x14ac:dyDescent="0.3">
       <c r="G58" s="17"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
       <c r="L58" s="13"/>
       <c r="M58" s="13"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="21"/>
-      <c r="P58" s="13"/>
-      <c r="T58" s="13"/>
-      <c r="U58" s="13"/>
-      <c r="V58" s="18"/>
-      <c r="X58" s="14"/>
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
-      <c r="AB58" s="18"/>
-      <c r="AC58" s="18"/>
-      <c r="AD58" s="18"/>
-      <c r="AE58" s="19"/>
-      <c r="AF58" s="16"/>
-      <c r="AG58" s="16"/>
-      <c r="AH58" s="16"/>
-      <c r="AI58" s="16"/>
-      <c r="AJ58" s="16"/>
-      <c r="AK58" s="16"/>
-      <c r="AL58" s="16"/>
-      <c r="AM58" s="16"/>
-      <c r="AN58" s="16"/>
-      <c r="AO58" s="16"/>
-    </row>
-    <row r="59" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G59" s="17"/>
+      <c r="AF58" s="12"/>
+      <c r="AG58" s="12"/>
+      <c r="AH58" s="12"/>
+      <c r="AI58" s="12"/>
+      <c r="AJ58" s="12"/>
+    </row>
+    <row r="59" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C59" s="13"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
       <c r="L59" s="13"/>
@@ -2221,8 +2231,7 @@
       <c r="AI59" s="12"/>
       <c r="AJ59" s="12"/>
     </row>
-    <row r="60" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C60" s="13"/>
+    <row r="60" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
       <c r="L60" s="13"/>
@@ -2235,7 +2244,7 @@
       <c r="AI60" s="12"/>
       <c r="AJ60" s="12"/>
     </row>
-    <row r="61" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
       <c r="L61" s="13"/>
@@ -2248,7 +2257,9 @@
       <c r="AI61" s="12"/>
       <c r="AJ61" s="12"/>
     </row>
-    <row r="62" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C62" s="13"/>
+      <c r="G62" s="17"/>
       <c r="I62" s="12"/>
       <c r="J62" s="12"/>
       <c r="L62" s="13"/>
@@ -2261,9 +2272,7 @@
       <c r="AI62" s="12"/>
       <c r="AJ62" s="12"/>
     </row>
-    <row r="63" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C63" s="13"/>
-      <c r="G63" s="17"/>
+    <row r="63" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I63" s="12"/>
       <c r="J63" s="12"/>
       <c r="L63" s="13"/>
@@ -2276,7 +2285,7 @@
       <c r="AI63" s="12"/>
       <c r="AJ63" s="12"/>
     </row>
-    <row r="64" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I64" s="12"/>
       <c r="J64" s="12"/>
       <c r="L64" s="13"/>
@@ -2289,51 +2298,51 @@
       <c r="AI64" s="12"/>
       <c r="AJ64" s="12"/>
     </row>
-    <row r="65" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C65" s="13"/>
+      <c r="G65" s="17"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
       <c r="L65" s="13"/>
       <c r="M65" s="13"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="21"/>
+      <c r="P65" s="13"/>
+      <c r="T65" s="13"/>
+      <c r="U65" s="13"/>
+      <c r="V65" s="18"/>
+      <c r="X65" s="14"/>
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
-      <c r="AF65" s="12"/>
-      <c r="AG65" s="12"/>
-      <c r="AH65" s="12"/>
-      <c r="AI65" s="12"/>
-      <c r="AJ65" s="12"/>
-    </row>
-    <row r="66" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C66" s="13"/>
-      <c r="G66" s="17"/>
+      <c r="AB65" s="18"/>
+      <c r="AC65" s="18"/>
+      <c r="AD65" s="18"/>
+      <c r="AE65" s="19"/>
+      <c r="AF65" s="16"/>
+      <c r="AG65" s="16"/>
+      <c r="AH65" s="16"/>
+      <c r="AI65" s="16"/>
+      <c r="AJ65" s="16"/>
+      <c r="AK65" s="16"/>
+      <c r="AL65" s="16"/>
+      <c r="AM65" s="16"/>
+      <c r="AN65" s="16"/>
+      <c r="AO65" s="16"/>
+    </row>
+    <row r="66" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I66" s="12"/>
       <c r="J66" s="12"/>
       <c r="L66" s="13"/>
       <c r="M66" s="13"/>
-      <c r="N66" s="18"/>
-      <c r="O66" s="21"/>
-      <c r="P66" s="13"/>
-      <c r="T66" s="13"/>
-      <c r="U66" s="13"/>
-      <c r="V66" s="18"/>
-      <c r="X66" s="14"/>
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
-      <c r="AB66" s="18"/>
-      <c r="AC66" s="18"/>
-      <c r="AD66" s="18"/>
-      <c r="AE66" s="19"/>
-      <c r="AF66" s="16"/>
-      <c r="AG66" s="16"/>
-      <c r="AH66" s="16"/>
-      <c r="AI66" s="16"/>
-      <c r="AJ66" s="16"/>
-      <c r="AK66" s="16"/>
-      <c r="AL66" s="16"/>
-      <c r="AM66" s="16"/>
-      <c r="AN66" s="16"/>
-      <c r="AO66" s="16"/>
-    </row>
-    <row r="67" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AF66" s="12"/>
+      <c r="AG66" s="12"/>
+      <c r="AH66" s="12"/>
+      <c r="AI66" s="12"/>
+      <c r="AJ66" s="12"/>
+    </row>
+    <row r="67" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
       <c r="L67" s="13"/>
@@ -2346,7 +2355,8 @@
       <c r="AI67" s="12"/>
       <c r="AJ67" s="12"/>
     </row>
-    <row r="68" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C68" s="13"/>
       <c r="I68" s="12"/>
       <c r="J68" s="12"/>
       <c r="L68" s="13"/>
@@ -2359,8 +2369,7 @@
       <c r="AI68" s="12"/>
       <c r="AJ68" s="12"/>
     </row>
-    <row r="69" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C69" s="13"/>
+    <row r="69" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I69" s="12"/>
       <c r="J69" s="12"/>
       <c r="L69" s="13"/>
@@ -2373,7 +2382,7 @@
       <c r="AI69" s="12"/>
       <c r="AJ69" s="12"/>
     </row>
-    <row r="70" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I70" s="12"/>
       <c r="J70" s="12"/>
       <c r="L70" s="13"/>
@@ -2386,7 +2395,8 @@
       <c r="AI70" s="12"/>
       <c r="AJ70" s="12"/>
     </row>
-    <row r="71" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C71" s="13"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
       <c r="L71" s="13"/>
@@ -2399,8 +2409,7 @@
       <c r="AI71" s="12"/>
       <c r="AJ71" s="12"/>
     </row>
-    <row r="72" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C72" s="13"/>
+    <row r="72" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
       <c r="L72" s="13"/>
@@ -2413,51 +2422,51 @@
       <c r="AI72" s="12"/>
       <c r="AJ72" s="12"/>
     </row>
-    <row r="73" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G73" s="17"/>
       <c r="I73" s="12"/>
       <c r="J73" s="12"/>
       <c r="L73" s="13"/>
       <c r="M73" s="13"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+      <c r="T73" s="13"/>
+      <c r="U73" s="13"/>
+      <c r="V73" s="18"/>
+      <c r="X73" s="14"/>
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
-      <c r="AF73" s="12"/>
-      <c r="AG73" s="12"/>
-      <c r="AH73" s="12"/>
-      <c r="AI73" s="12"/>
-      <c r="AJ73" s="12"/>
-    </row>
-    <row r="74" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G74" s="17"/>
+      <c r="AB73" s="18"/>
+      <c r="AC73" s="18"/>
+      <c r="AD73" s="18"/>
+      <c r="AE73" s="19"/>
+      <c r="AF73" s="16"/>
+      <c r="AG73" s="16"/>
+      <c r="AH73" s="16"/>
+      <c r="AI73" s="16"/>
+      <c r="AJ73" s="16"/>
+      <c r="AK73" s="16"/>
+      <c r="AL73" s="16"/>
+      <c r="AM73" s="16"/>
+      <c r="AN73" s="16"/>
+      <c r="AO73" s="16"/>
+    </row>
+    <row r="74" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C74" s="13"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
       <c r="L74" s="13"/>
       <c r="M74" s="13"/>
-      <c r="N74" s="18"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="T74" s="13"/>
-      <c r="U74" s="13"/>
-      <c r="V74" s="18"/>
-      <c r="X74" s="14"/>
       <c r="Y74" s="14"/>
       <c r="Z74" s="14"/>
-      <c r="AB74" s="18"/>
-      <c r="AC74" s="18"/>
-      <c r="AD74" s="18"/>
-      <c r="AE74" s="19"/>
-      <c r="AF74" s="16"/>
-      <c r="AG74" s="16"/>
-      <c r="AH74" s="16"/>
-      <c r="AI74" s="16"/>
-      <c r="AJ74" s="16"/>
-      <c r="AK74" s="16"/>
-      <c r="AL74" s="16"/>
-      <c r="AM74" s="16"/>
-      <c r="AN74" s="16"/>
-      <c r="AO74" s="16"/>
-    </row>
-    <row r="75" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C75" s="13"/>
+      <c r="AF74" s="12"/>
+      <c r="AG74" s="12"/>
+      <c r="AH74" s="12"/>
+      <c r="AI74" s="12"/>
+      <c r="AJ74" s="12"/>
+    </row>
+    <row r="75" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I75" s="12"/>
       <c r="J75" s="12"/>
       <c r="L75" s="13"/>
@@ -2470,7 +2479,7 @@
       <c r="AI75" s="12"/>
       <c r="AJ75" s="12"/>
     </row>
-    <row r="76" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I76" s="12"/>
       <c r="J76" s="12"/>
       <c r="L76" s="13"/>
@@ -2483,51 +2492,51 @@
       <c r="AI76" s="12"/>
       <c r="AJ76" s="12"/>
     </row>
-    <row r="77" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G77" s="17"/>
       <c r="I77" s="12"/>
       <c r="J77" s="12"/>
       <c r="L77" s="13"/>
       <c r="M77" s="13"/>
+      <c r="N77" s="18"/>
+      <c r="O77" s="21"/>
+      <c r="P77" s="13"/>
+      <c r="T77" s="13"/>
+      <c r="U77" s="13"/>
+      <c r="V77" s="18"/>
+      <c r="X77" s="14"/>
       <c r="Y77" s="14"/>
       <c r="Z77" s="14"/>
+      <c r="AB77" s="18"/>
+      <c r="AC77" s="18"/>
+      <c r="AD77" s="18"/>
+      <c r="AE77" s="19"/>
       <c r="AF77" s="12"/>
-      <c r="AG77" s="12"/>
-      <c r="AH77" s="12"/>
-      <c r="AI77" s="12"/>
-      <c r="AJ77" s="12"/>
-    </row>
-    <row r="78" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G78" s="17"/>
+      <c r="AG77" s="16"/>
+      <c r="AH77" s="16"/>
+      <c r="AI77" s="16"/>
+      <c r="AJ77" s="16"/>
+      <c r="AK77" s="16"/>
+      <c r="AL77" s="16"/>
+      <c r="AM77" s="16"/>
+      <c r="AN77" s="16"/>
+      <c r="AO77" s="16"/>
+    </row>
+    <row r="78" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C78" s="13"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
       <c r="L78" s="13"/>
       <c r="M78" s="13"/>
-      <c r="N78" s="18"/>
-      <c r="O78" s="21"/>
-      <c r="P78" s="13"/>
-      <c r="T78" s="13"/>
-      <c r="U78" s="13"/>
-      <c r="V78" s="18"/>
-      <c r="X78" s="14"/>
       <c r="Y78" s="14"/>
       <c r="Z78" s="14"/>
-      <c r="AB78" s="18"/>
-      <c r="AC78" s="18"/>
-      <c r="AD78" s="18"/>
-      <c r="AE78" s="19"/>
       <c r="AF78" s="12"/>
-      <c r="AG78" s="16"/>
-      <c r="AH78" s="16"/>
-      <c r="AI78" s="16"/>
-      <c r="AJ78" s="16"/>
-      <c r="AK78" s="16"/>
-      <c r="AL78" s="16"/>
-      <c r="AM78" s="16"/>
-      <c r="AN78" s="16"/>
-      <c r="AO78" s="16"/>
-    </row>
-    <row r="79" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C79" s="13"/>
+      <c r="AG78" s="12"/>
+      <c r="AH78" s="12"/>
+      <c r="AI78" s="12"/>
+      <c r="AJ78" s="12"/>
+    </row>
+    <row r="79" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
       <c r="L79" s="13"/>
@@ -2540,7 +2549,7 @@
       <c r="AI79" s="12"/>
       <c r="AJ79" s="12"/>
     </row>
-    <row r="80" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
       <c r="L80" s="13"/>
@@ -2553,7 +2562,7 @@
       <c r="AI80" s="12"/>
       <c r="AJ80" s="12"/>
     </row>
-    <row r="81" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I81" s="12"/>
       <c r="J81" s="12"/>
       <c r="L81" s="13"/>
@@ -2566,7 +2575,8 @@
       <c r="AI81" s="12"/>
       <c r="AJ81" s="12"/>
     </row>
-    <row r="82" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C82" s="13"/>
       <c r="I82" s="12"/>
       <c r="J82" s="12"/>
       <c r="L82" s="13"/>
@@ -2579,8 +2589,7 @@
       <c r="AI82" s="12"/>
       <c r="AJ82" s="12"/>
     </row>
-    <row r="83" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C83" s="13"/>
+    <row r="83" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
       <c r="L83" s="13"/>
@@ -2593,7 +2602,7 @@
       <c r="AI83" s="12"/>
       <c r="AJ83" s="12"/>
     </row>
-    <row r="84" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
       <c r="L84" s="13"/>
@@ -2606,7 +2615,7 @@
       <c r="AI84" s="12"/>
       <c r="AJ84" s="12"/>
     </row>
-    <row r="85" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I85" s="12"/>
       <c r="J85" s="12"/>
       <c r="L85" s="13"/>
@@ -2619,7 +2628,8 @@
       <c r="AI85" s="12"/>
       <c r="AJ85" s="12"/>
     </row>
-    <row r="86" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C86" s="13"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
       <c r="L86" s="13"/>
@@ -2632,8 +2642,7 @@
       <c r="AI86" s="12"/>
       <c r="AJ86" s="12"/>
     </row>
-    <row r="87" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C87" s="13"/>
+    <row r="87" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
       <c r="L87" s="13"/>
@@ -2646,50 +2655,51 @@
       <c r="AI87" s="12"/>
       <c r="AJ87" s="12"/>
     </row>
-    <row r="88" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G88" s="17"/>
       <c r="I88" s="12"/>
       <c r="J88" s="12"/>
       <c r="L88" s="13"/>
       <c r="M88" s="13"/>
+      <c r="N88" s="18"/>
+      <c r="O88" s="13"/>
+      <c r="P88" s="13"/>
+      <c r="T88" s="13"/>
+      <c r="U88" s="13"/>
+      <c r="V88" s="18"/>
+      <c r="X88" s="14"/>
       <c r="Y88" s="14"/>
       <c r="Z88" s="14"/>
+      <c r="AB88" s="18"/>
+      <c r="AC88" s="18"/>
+      <c r="AD88" s="18"/>
+      <c r="AE88" s="19"/>
       <c r="AF88" s="12"/>
-      <c r="AG88" s="12"/>
-      <c r="AH88" s="12"/>
-      <c r="AI88" s="12"/>
-      <c r="AJ88" s="12"/>
-    </row>
-    <row r="89" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G89" s="17"/>
+      <c r="AG88" s="16"/>
+      <c r="AH88" s="16"/>
+      <c r="AI88" s="16"/>
+      <c r="AJ88" s="16"/>
+      <c r="AK88" s="16"/>
+      <c r="AL88" s="16"/>
+      <c r="AM88" s="16"/>
+      <c r="AN88" s="16"/>
+      <c r="AO88" s="16"/>
+    </row>
+    <row r="89" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I89" s="12"/>
       <c r="J89" s="12"/>
       <c r="L89" s="13"/>
       <c r="M89" s="13"/>
-      <c r="N89" s="18"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="13"/>
-      <c r="T89" s="13"/>
-      <c r="U89" s="13"/>
-      <c r="V89" s="18"/>
-      <c r="X89" s="14"/>
       <c r="Y89" s="14"/>
       <c r="Z89" s="14"/>
-      <c r="AB89" s="18"/>
-      <c r="AC89" s="18"/>
-      <c r="AD89" s="18"/>
-      <c r="AE89" s="19"/>
       <c r="AF89" s="12"/>
-      <c r="AG89" s="16"/>
-      <c r="AH89" s="16"/>
-      <c r="AI89" s="16"/>
-      <c r="AJ89" s="16"/>
-      <c r="AK89" s="16"/>
-      <c r="AL89" s="16"/>
-      <c r="AM89" s="16"/>
-      <c r="AN89" s="16"/>
-      <c r="AO89" s="16"/>
-    </row>
-    <row r="90" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AG89" s="12"/>
+      <c r="AH89" s="12"/>
+      <c r="AI89" s="12"/>
+      <c r="AJ89" s="12"/>
+    </row>
+    <row r="90" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C90" s="13"/>
       <c r="I90" s="12"/>
       <c r="J90" s="12"/>
       <c r="L90" s="13"/>
@@ -2702,8 +2712,7 @@
       <c r="AI90" s="12"/>
       <c r="AJ90" s="12"/>
     </row>
-    <row r="91" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C91" s="13"/>
+    <row r="91" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I91" s="12"/>
       <c r="J91" s="12"/>
       <c r="L91" s="13"/>
@@ -2716,7 +2725,7 @@
       <c r="AI91" s="12"/>
       <c r="AJ91" s="12"/>
     </row>
-    <row r="92" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I92" s="12"/>
       <c r="J92" s="12"/>
       <c r="L92" s="13"/>
@@ -2729,7 +2738,7 @@
       <c r="AI92" s="12"/>
       <c r="AJ92" s="12"/>
     </row>
-    <row r="93" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I93" s="12"/>
       <c r="J93" s="12"/>
       <c r="L93" s="13"/>
@@ -2742,7 +2751,8 @@
       <c r="AI93" s="12"/>
       <c r="AJ93" s="12"/>
     </row>
-    <row r="94" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C94" s="13"/>
       <c r="I94" s="12"/>
       <c r="J94" s="12"/>
       <c r="L94" s="13"/>
@@ -2755,8 +2765,7 @@
       <c r="AI94" s="12"/>
       <c r="AJ94" s="12"/>
     </row>
-    <row r="95" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C95" s="13"/>
+    <row r="95" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I95" s="12"/>
       <c r="J95" s="12"/>
       <c r="L95" s="13"/>
@@ -2769,50 +2778,51 @@
       <c r="AI95" s="12"/>
       <c r="AJ95" s="12"/>
     </row>
-    <row r="96" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G96" s="17"/>
       <c r="I96" s="12"/>
       <c r="J96" s="12"/>
       <c r="L96" s="13"/>
       <c r="M96" s="13"/>
+      <c r="N96" s="18"/>
+      <c r="O96" s="13"/>
+      <c r="P96" s="13"/>
+      <c r="T96" s="13"/>
+      <c r="U96" s="13"/>
+      <c r="V96" s="18"/>
+      <c r="X96" s="14"/>
       <c r="Y96" s="14"/>
       <c r="Z96" s="14"/>
+      <c r="AB96" s="18"/>
+      <c r="AC96" s="18"/>
+      <c r="AD96" s="18"/>
+      <c r="AE96" s="19"/>
       <c r="AF96" s="12"/>
-      <c r="AG96" s="12"/>
-      <c r="AH96" s="12"/>
-      <c r="AI96" s="12"/>
-      <c r="AJ96" s="12"/>
-    </row>
-    <row r="97" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G97" s="17"/>
+      <c r="AG96" s="16"/>
+      <c r="AH96" s="16"/>
+      <c r="AI96" s="16"/>
+      <c r="AJ96" s="16"/>
+      <c r="AK96" s="16"/>
+      <c r="AL96" s="16"/>
+      <c r="AM96" s="16"/>
+      <c r="AN96" s="16"/>
+      <c r="AO96" s="16"/>
+    </row>
+    <row r="97" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I97" s="12"/>
       <c r="J97" s="12"/>
       <c r="L97" s="13"/>
       <c r="M97" s="13"/>
-      <c r="N97" s="18"/>
-      <c r="O97" s="13"/>
-      <c r="P97" s="13"/>
-      <c r="T97" s="13"/>
-      <c r="U97" s="13"/>
-      <c r="V97" s="18"/>
-      <c r="X97" s="14"/>
       <c r="Y97" s="14"/>
       <c r="Z97" s="14"/>
-      <c r="AB97" s="18"/>
-      <c r="AC97" s="18"/>
-      <c r="AD97" s="18"/>
-      <c r="AE97" s="19"/>
       <c r="AF97" s="12"/>
-      <c r="AG97" s="16"/>
-      <c r="AH97" s="16"/>
-      <c r="AI97" s="16"/>
-      <c r="AJ97" s="16"/>
-      <c r="AK97" s="16"/>
-      <c r="AL97" s="16"/>
-      <c r="AM97" s="16"/>
-      <c r="AN97" s="16"/>
-      <c r="AO97" s="16"/>
-    </row>
-    <row r="98" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AG97" s="12"/>
+      <c r="AH97" s="12"/>
+      <c r="AI97" s="12"/>
+      <c r="AJ97" s="12"/>
+    </row>
+    <row r="98" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C98" s="13"/>
       <c r="I98" s="12"/>
       <c r="J98" s="12"/>
       <c r="L98" s="13"/>
@@ -2825,8 +2835,7 @@
       <c r="AI98" s="12"/>
       <c r="AJ98" s="12"/>
     </row>
-    <row r="99" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C99" s="13"/>
+    <row r="99" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I99" s="12"/>
       <c r="J99" s="12"/>
       <c r="L99" s="13"/>
@@ -2839,7 +2848,7 @@
       <c r="AI99" s="12"/>
       <c r="AJ99" s="12"/>
     </row>
-    <row r="100" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I100" s="12"/>
       <c r="J100" s="12"/>
       <c r="L100" s="13"/>
@@ -2852,7 +2861,7 @@
       <c r="AI100" s="12"/>
       <c r="AJ100" s="12"/>
     </row>
-    <row r="101" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I101" s="12"/>
       <c r="J101" s="12"/>
       <c r="L101" s="13"/>
@@ -2865,7 +2874,8 @@
       <c r="AI101" s="12"/>
       <c r="AJ101" s="12"/>
     </row>
-    <row r="102" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C102" s="13"/>
       <c r="I102" s="12"/>
       <c r="J102" s="12"/>
       <c r="L102" s="13"/>
@@ -2878,8 +2888,7 @@
       <c r="AI102" s="12"/>
       <c r="AJ102" s="12"/>
     </row>
-    <row r="103" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C103" s="13"/>
+    <row r="103" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I103" s="12"/>
       <c r="J103" s="12"/>
       <c r="L103" s="13"/>
@@ -2892,7 +2901,7 @@
       <c r="AI103" s="12"/>
       <c r="AJ103" s="12"/>
     </row>
-    <row r="104" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I104" s="12"/>
       <c r="J104" s="12"/>
       <c r="L104" s="13"/>
@@ -2905,51 +2914,51 @@
       <c r="AI104" s="12"/>
       <c r="AJ104" s="12"/>
     </row>
-    <row r="105" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G105" s="17"/>
       <c r="I105" s="12"/>
       <c r="J105" s="12"/>
       <c r="L105" s="13"/>
       <c r="M105" s="13"/>
+      <c r="N105" s="18"/>
+      <c r="O105" s="13"/>
+      <c r="P105" s="13"/>
+      <c r="T105" s="13"/>
+      <c r="U105" s="13"/>
+      <c r="V105" s="18"/>
+      <c r="X105" s="14"/>
       <c r="Y105" s="14"/>
       <c r="Z105" s="14"/>
+      <c r="AB105" s="18"/>
+      <c r="AC105" s="18"/>
+      <c r="AD105" s="18"/>
+      <c r="AE105" s="19"/>
       <c r="AF105" s="12"/>
-      <c r="AG105" s="12"/>
-      <c r="AH105" s="12"/>
-      <c r="AI105" s="12"/>
-      <c r="AJ105" s="12"/>
-    </row>
-    <row r="106" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G106" s="17"/>
+      <c r="AG105" s="16"/>
+      <c r="AH105" s="16"/>
+      <c r="AI105" s="16"/>
+      <c r="AJ105" s="16"/>
+      <c r="AK105" s="16"/>
+      <c r="AL105" s="16"/>
+      <c r="AM105" s="16"/>
+      <c r="AN105" s="16"/>
+      <c r="AO105" s="16"/>
+    </row>
+    <row r="106" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C106" s="13"/>
       <c r="I106" s="12"/>
       <c r="J106" s="12"/>
       <c r="L106" s="13"/>
       <c r="M106" s="13"/>
-      <c r="N106" s="18"/>
-      <c r="O106" s="13"/>
-      <c r="P106" s="13"/>
-      <c r="T106" s="13"/>
-      <c r="U106" s="13"/>
-      <c r="V106" s="18"/>
-      <c r="X106" s="14"/>
       <c r="Y106" s="14"/>
       <c r="Z106" s="14"/>
-      <c r="AB106" s="18"/>
-      <c r="AC106" s="18"/>
-      <c r="AD106" s="18"/>
-      <c r="AE106" s="19"/>
       <c r="AF106" s="12"/>
-      <c r="AG106" s="16"/>
-      <c r="AH106" s="16"/>
-      <c r="AI106" s="16"/>
-      <c r="AJ106" s="16"/>
-      <c r="AK106" s="16"/>
-      <c r="AL106" s="16"/>
-      <c r="AM106" s="16"/>
-      <c r="AN106" s="16"/>
-      <c r="AO106" s="16"/>
-    </row>
-    <row r="107" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C107" s="13"/>
+      <c r="AG106" s="12"/>
+      <c r="AH106" s="12"/>
+      <c r="AI106" s="12"/>
+      <c r="AJ106" s="12"/>
+    </row>
+    <row r="107" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I107" s="12"/>
       <c r="J107" s="12"/>
       <c r="L107" s="13"/>
@@ -2962,7 +2971,7 @@
       <c r="AI107" s="12"/>
       <c r="AJ107" s="12"/>
     </row>
-    <row r="108" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I108" s="12"/>
       <c r="J108" s="12"/>
       <c r="L108" s="13"/>
@@ -2975,7 +2984,7 @@
       <c r="AI108" s="12"/>
       <c r="AJ108" s="12"/>
     </row>
-    <row r="109" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I109" s="12"/>
       <c r="J109" s="12"/>
       <c r="L109" s="13"/>
@@ -2988,7 +2997,8 @@
       <c r="AI109" s="12"/>
       <c r="AJ109" s="12"/>
     </row>
-    <row r="110" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C110" s="13"/>
       <c r="I110" s="12"/>
       <c r="J110" s="12"/>
       <c r="L110" s="13"/>
@@ -3001,8 +3011,7 @@
       <c r="AI110" s="12"/>
       <c r="AJ110" s="12"/>
     </row>
-    <row r="111" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C111" s="13"/>
+    <row r="111" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I111" s="12"/>
       <c r="J111" s="12"/>
       <c r="L111" s="13"/>
@@ -3015,7 +3024,7 @@
       <c r="AI111" s="12"/>
       <c r="AJ111" s="12"/>
     </row>
-    <row r="112" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I112" s="12"/>
       <c r="J112" s="12"/>
       <c r="L112" s="13"/>
@@ -3028,54 +3037,54 @@
       <c r="AI112" s="12"/>
       <c r="AJ112" s="12"/>
     </row>
-    <row r="113" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I113" s="12"/>
       <c r="J113" s="12"/>
       <c r="L113" s="13"/>
       <c r="M113" s="13"/>
       <c r="Y113" s="14"/>
       <c r="Z113" s="14"/>
+      <c r="AB113" s="18"/>
+      <c r="AC113" s="18"/>
+      <c r="AD113" s="18"/>
+      <c r="AE113" s="19"/>
       <c r="AF113" s="12"/>
-      <c r="AG113" s="12"/>
-      <c r="AH113" s="12"/>
-      <c r="AI113" s="12"/>
-      <c r="AJ113" s="12"/>
-    </row>
-    <row r="114" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AG113" s="16"/>
+      <c r="AH113" s="16"/>
+      <c r="AI113" s="16"/>
+      <c r="AJ113" s="16"/>
+      <c r="AK113" s="16"/>
+      <c r="AL113" s="16"/>
+      <c r="AM113" s="16"/>
+      <c r="AN113" s="16"/>
+      <c r="AO113" s="16"/>
+    </row>
+    <row r="114" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C114" s="13"/>
       <c r="I114" s="12"/>
       <c r="J114" s="12"/>
       <c r="L114" s="13"/>
       <c r="M114" s="13"/>
+      <c r="N114" s="18"/>
+      <c r="O114" s="13"/>
+      <c r="P114" s="13"/>
+      <c r="T114" s="13"/>
+      <c r="U114" s="13"/>
+      <c r="V114" s="18"/>
+      <c r="X114" s="14"/>
       <c r="Y114" s="14"/>
       <c r="Z114" s="14"/>
-      <c r="AB114" s="18"/>
-      <c r="AC114" s="18"/>
-      <c r="AD114" s="18"/>
-      <c r="AE114" s="19"/>
       <c r="AF114" s="12"/>
-      <c r="AG114" s="16"/>
-      <c r="AH114" s="16"/>
-      <c r="AI114" s="16"/>
-      <c r="AJ114" s="16"/>
-      <c r="AK114" s="16"/>
-      <c r="AL114" s="16"/>
-      <c r="AM114" s="16"/>
-      <c r="AN114" s="16"/>
-      <c r="AO114" s="16"/>
-    </row>
-    <row r="115" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C115" s="13"/>
+      <c r="AG114" s="12"/>
+      <c r="AH114" s="12"/>
+      <c r="AI114" s="12"/>
+      <c r="AJ114" s="12"/>
+    </row>
+    <row r="115" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I115" s="12"/>
       <c r="J115" s="12"/>
       <c r="L115" s="13"/>
       <c r="M115" s="13"/>
-      <c r="N115" s="18"/>
-      <c r="O115" s="13"/>
-      <c r="P115" s="13"/>
-      <c r="T115" s="13"/>
-      <c r="U115" s="13"/>
-      <c r="V115" s="18"/>
-      <c r="X115" s="14"/>
       <c r="Y115" s="14"/>
       <c r="Z115" s="14"/>
       <c r="AF115" s="12"/>
@@ -3084,7 +3093,7 @@
       <c r="AI115" s="12"/>
       <c r="AJ115" s="12"/>
     </row>
-    <row r="116" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I116" s="12"/>
       <c r="J116" s="12"/>
       <c r="L116" s="13"/>
@@ -3097,7 +3106,7 @@
       <c r="AI116" s="12"/>
       <c r="AJ116" s="12"/>
     </row>
-    <row r="117" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I117" s="12"/>
       <c r="J117" s="12"/>
       <c r="L117" s="13"/>
@@ -3110,7 +3119,8 @@
       <c r="AI117" s="12"/>
       <c r="AJ117" s="12"/>
     </row>
-    <row r="118" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C118" s="13"/>
       <c r="I118" s="12"/>
       <c r="J118" s="12"/>
       <c r="L118" s="13"/>
@@ -3123,8 +3133,7 @@
       <c r="AI118" s="12"/>
       <c r="AJ118" s="12"/>
     </row>
-    <row r="119" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C119" s="13"/>
+    <row r="119" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I119" s="12"/>
       <c r="J119" s="12"/>
       <c r="L119" s="13"/>
@@ -3137,7 +3146,7 @@
       <c r="AI119" s="12"/>
       <c r="AJ119" s="12"/>
     </row>
-    <row r="120" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I120" s="12"/>
       <c r="J120" s="12"/>
       <c r="L120" s="13"/>
@@ -3150,7 +3159,7 @@
       <c r="AI120" s="12"/>
       <c r="AJ120" s="12"/>
     </row>
-    <row r="121" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I121" s="12"/>
       <c r="J121" s="12"/>
       <c r="L121" s="13"/>
@@ -3163,7 +3172,8 @@
       <c r="AI121" s="12"/>
       <c r="AJ121" s="12"/>
     </row>
-    <row r="122" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C122" s="13"/>
       <c r="I122" s="12"/>
       <c r="J122" s="12"/>
       <c r="L122" s="13"/>
@@ -3176,51 +3186,50 @@
       <c r="AI122" s="12"/>
       <c r="AJ122" s="12"/>
     </row>
-    <row r="123" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C123" s="13"/>
+    <row r="123" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G123" s="17"/>
       <c r="I123" s="12"/>
       <c r="J123" s="12"/>
       <c r="L123" s="13"/>
       <c r="M123" s="13"/>
+      <c r="N123" s="18"/>
+      <c r="O123" s="21"/>
+      <c r="P123" s="13"/>
+      <c r="T123" s="13"/>
+      <c r="U123" s="13"/>
+      <c r="V123" s="18"/>
+      <c r="X123" s="14"/>
       <c r="Y123" s="14"/>
       <c r="Z123" s="14"/>
+      <c r="AB123" s="18"/>
+      <c r="AC123" s="18"/>
+      <c r="AD123" s="18"/>
+      <c r="AE123" s="19"/>
       <c r="AF123" s="12"/>
-      <c r="AG123" s="12"/>
-      <c r="AH123" s="12"/>
-      <c r="AI123" s="12"/>
-      <c r="AJ123" s="12"/>
-    </row>
-    <row r="124" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G124" s="17"/>
+      <c r="AG123" s="16"/>
+      <c r="AH123" s="16"/>
+      <c r="AI123" s="16"/>
+      <c r="AJ123" s="16"/>
+      <c r="AK123" s="16"/>
+      <c r="AL123" s="16"/>
+      <c r="AM123" s="16"/>
+      <c r="AN123" s="16"/>
+      <c r="AO123" s="16"/>
+    </row>
+    <row r="124" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I124" s="12"/>
       <c r="J124" s="12"/>
       <c r="L124" s="13"/>
       <c r="M124" s="13"/>
-      <c r="N124" s="18"/>
-      <c r="O124" s="21"/>
-      <c r="P124" s="13"/>
-      <c r="T124" s="13"/>
-      <c r="U124" s="13"/>
-      <c r="V124" s="18"/>
-      <c r="X124" s="14"/>
       <c r="Y124" s="14"/>
       <c r="Z124" s="14"/>
-      <c r="AB124" s="18"/>
-      <c r="AC124" s="18"/>
-      <c r="AD124" s="18"/>
-      <c r="AE124" s="19"/>
       <c r="AF124" s="12"/>
-      <c r="AG124" s="16"/>
-      <c r="AH124" s="16"/>
-      <c r="AI124" s="16"/>
-      <c r="AJ124" s="16"/>
-      <c r="AK124" s="16"/>
-      <c r="AL124" s="16"/>
-      <c r="AM124" s="16"/>
-      <c r="AN124" s="16"/>
-      <c r="AO124" s="16"/>
-    </row>
-    <row r="125" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AG124" s="12"/>
+      <c r="AH124" s="12"/>
+      <c r="AI124" s="12"/>
+      <c r="AJ124" s="12"/>
+    </row>
+    <row r="125" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I125" s="12"/>
       <c r="J125" s="12"/>
       <c r="L125" s="13"/>
@@ -3233,21 +3242,21 @@
       <c r="AI125" s="12"/>
       <c r="AJ125" s="12"/>
     </row>
-    <row r="126" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C126" s="13"/>
       <c r="I126" s="12"/>
       <c r="J126" s="12"/>
       <c r="L126" s="13"/>
       <c r="M126" s="13"/>
       <c r="Y126" s="14"/>
       <c r="Z126" s="14"/>
-      <c r="AF126" s="12"/>
+      <c r="AF126" s="16"/>
       <c r="AG126" s="12"/>
       <c r="AH126" s="12"/>
       <c r="AI126" s="12"/>
       <c r="AJ126" s="12"/>
     </row>
-    <row r="127" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C127" s="13"/>
+    <row r="127" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I127" s="12"/>
       <c r="J127" s="12"/>
       <c r="L127" s="13"/>
@@ -3260,7 +3269,7 @@
       <c r="AI127" s="12"/>
       <c r="AJ127" s="12"/>
     </row>
-    <row r="128" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I128" s="12"/>
       <c r="J128" s="12"/>
       <c r="L128" s="13"/>
@@ -3273,7 +3282,7 @@
       <c r="AI128" s="12"/>
       <c r="AJ128" s="12"/>
     </row>
-    <row r="129" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I129" s="12"/>
       <c r="J129" s="12"/>
       <c r="L129" s="13"/>
@@ -3286,7 +3295,8 @@
       <c r="AI129" s="12"/>
       <c r="AJ129" s="12"/>
     </row>
-    <row r="130" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C130" s="13"/>
       <c r="I130" s="12"/>
       <c r="J130" s="12"/>
       <c r="L130" s="13"/>
@@ -3299,8 +3309,7 @@
       <c r="AI130" s="12"/>
       <c r="AJ130" s="12"/>
     </row>
-    <row r="131" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C131" s="13"/>
+    <row r="131" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I131" s="12"/>
       <c r="J131" s="12"/>
       <c r="L131" s="13"/>
@@ -3313,50 +3322,51 @@
       <c r="AI131" s="12"/>
       <c r="AJ131" s="12"/>
     </row>
-    <row r="132" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G132" s="17"/>
       <c r="I132" s="12"/>
       <c r="J132" s="12"/>
       <c r="L132" s="13"/>
       <c r="M132" s="13"/>
+      <c r="N132" s="18"/>
+      <c r="O132" s="21"/>
+      <c r="P132" s="13"/>
+      <c r="T132" s="13"/>
+      <c r="U132" s="13"/>
+      <c r="V132" s="18"/>
+      <c r="X132" s="14"/>
       <c r="Y132" s="14"/>
       <c r="Z132" s="14"/>
+      <c r="AB132" s="18"/>
+      <c r="AC132" s="18"/>
+      <c r="AD132" s="18"/>
+      <c r="AE132" s="19"/>
       <c r="AF132" s="16"/>
-      <c r="AG132" s="12"/>
-      <c r="AH132" s="12"/>
-      <c r="AI132" s="12"/>
-      <c r="AJ132" s="12"/>
-    </row>
-    <row r="133" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G133" s="17"/>
+      <c r="AG132" s="16"/>
+      <c r="AH132" s="16"/>
+      <c r="AI132" s="16"/>
+      <c r="AJ132" s="16"/>
+      <c r="AK132" s="16"/>
+      <c r="AL132" s="16"/>
+      <c r="AM132" s="16"/>
+      <c r="AN132" s="16"/>
+      <c r="AO132" s="16"/>
+    </row>
+    <row r="133" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I133" s="12"/>
       <c r="J133" s="12"/>
       <c r="L133" s="13"/>
       <c r="M133" s="13"/>
-      <c r="N133" s="18"/>
-      <c r="O133" s="21"/>
-      <c r="P133" s="13"/>
-      <c r="T133" s="13"/>
-      <c r="U133" s="13"/>
-      <c r="V133" s="18"/>
-      <c r="X133" s="14"/>
       <c r="Y133" s="14"/>
       <c r="Z133" s="14"/>
-      <c r="AB133" s="18"/>
-      <c r="AC133" s="18"/>
-      <c r="AD133" s="18"/>
-      <c r="AE133" s="19"/>
       <c r="AF133" s="16"/>
-      <c r="AG133" s="16"/>
-      <c r="AH133" s="16"/>
-      <c r="AI133" s="16"/>
-      <c r="AJ133" s="16"/>
-      <c r="AK133" s="16"/>
-      <c r="AL133" s="16"/>
-      <c r="AM133" s="16"/>
-      <c r="AN133" s="16"/>
-      <c r="AO133" s="16"/>
-    </row>
-    <row r="134" spans="3:41" x14ac:dyDescent="0.25">
+      <c r="AG133" s="12"/>
+      <c r="AH133" s="12"/>
+      <c r="AI133" s="12"/>
+      <c r="AJ133" s="12"/>
+    </row>
+    <row r="134" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C134" s="13"/>
       <c r="I134" s="12"/>
       <c r="J134" s="12"/>
       <c r="L134" s="13"/>
@@ -3369,8 +3379,7 @@
       <c r="AI134" s="12"/>
       <c r="AJ134" s="12"/>
     </row>
-    <row r="135" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C135" s="13"/>
+    <row r="135" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I135" s="12"/>
       <c r="J135" s="12"/>
       <c r="L135" s="13"/>
@@ -3383,7 +3392,7 @@
       <c r="AI135" s="12"/>
       <c r="AJ135" s="12"/>
     </row>
-    <row r="136" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I136" s="12"/>
       <c r="J136" s="12"/>
       <c r="L136" s="13"/>
@@ -3396,7 +3405,7 @@
       <c r="AI136" s="12"/>
       <c r="AJ136" s="12"/>
     </row>
-    <row r="137" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I137" s="12"/>
       <c r="J137" s="12"/>
       <c r="L137" s="13"/>
@@ -3409,7 +3418,8 @@
       <c r="AI137" s="12"/>
       <c r="AJ137" s="12"/>
     </row>
-    <row r="138" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="C138" s="13"/>
       <c r="I138" s="12"/>
       <c r="J138" s="12"/>
       <c r="L138" s="13"/>
@@ -3422,8 +3432,7 @@
       <c r="AI138" s="12"/>
       <c r="AJ138" s="12"/>
     </row>
-    <row r="139" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="C139" s="13"/>
+    <row r="139" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I139" s="12"/>
       <c r="J139" s="12"/>
       <c r="L139" s="13"/>
@@ -3436,7 +3445,7 @@
       <c r="AI139" s="12"/>
       <c r="AJ139" s="12"/>
     </row>
-    <row r="140" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:41" x14ac:dyDescent="0.3">
       <c r="I140" s="12"/>
       <c r="J140" s="12"/>
       <c r="L140" s="13"/>
@@ -3449,51 +3458,50 @@
       <c r="AI140" s="12"/>
       <c r="AJ140" s="12"/>
     </row>
-    <row r="141" spans="3:41" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:41" x14ac:dyDescent="0.3">
+      <c r="G141" s="17"/>
       <c r="I141" s="12"/>
       <c r="J141" s="12"/>
       <c r="L141" s="13"/>
       <c r="M141" s="13"/>
+      <c r="N141" s="18"/>
+      <c r="O141" s="21"/>
+      <c r="P141" s="13"/>
+      <c r="T141" s="13"/>
+      <c r="U141" s="13"/>
+      <c r="V141" s="18"/>
+      <c r="X141" s="14"/>
       <c r="Y141" s="14"/>
       <c r="Z141" s="14"/>
+      <c r="AB141" s="18"/>
+      <c r="AC141" s="18"/>
+      <c r="AD141" s="18"/>
+      <c r="AE141" s="19"/>
       <c r="AF141" s="16"/>
-      <c r="AG141" s="12"/>
-      <c r="AH141" s="12"/>
-      <c r="AI141" s="12"/>
-      <c r="AJ141" s="12"/>
-    </row>
-    <row r="142" spans="3:41" x14ac:dyDescent="0.25">
-      <c r="G142" s="17"/>
+      <c r="AG141" s="16"/>
+      <c r="AH141" s="16"/>
+      <c r="AI141" s="16"/>
+      <c r="AJ141" s="16"/>
+      <c r="AK141" s="16"/>
+      <c r="AL141" s="16"/>
+      <c r="AM141" s="16"/>
+      <c r="AN141" s="16"/>
+      <c r="AO141" s="16"/>
+    </row>
+    <row r="142" spans="3:41" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C142" s="13"/>
       <c r="I142" s="12"/>
       <c r="J142" s="12"/>
       <c r="L142" s="13"/>
       <c r="M142" s="13"/>
-      <c r="N142" s="18"/>
-      <c r="O142" s="21"/>
-      <c r="P142" s="13"/>
-      <c r="T142" s="13"/>
-      <c r="U142" s="13"/>
-      <c r="V142" s="18"/>
-      <c r="X142" s="14"/>
       <c r="Y142" s="14"/>
       <c r="Z142" s="14"/>
-      <c r="AB142" s="18"/>
-      <c r="AC142" s="18"/>
-      <c r="AD142" s="18"/>
-      <c r="AE142" s="19"/>
       <c r="AF142" s="16"/>
-      <c r="AG142" s="16"/>
-      <c r="AH142" s="16"/>
-      <c r="AI142" s="16"/>
-      <c r="AJ142" s="16"/>
-      <c r="AK142" s="16"/>
-      <c r="AL142" s="16"/>
-      <c r="AM142" s="16"/>
-      <c r="AN142" s="16"/>
-      <c r="AO142" s="16"/>
-    </row>
-    <row r="143" spans="3:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C143" s="13"/>
+      <c r="AG142" s="12"/>
+      <c r="AH142" s="12"/>
+      <c r="AI142" s="12"/>
+    </row>
+    <row r="143" spans="3:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="I143" s="12"/>
       <c r="J143" s="12"/>
       <c r="L143" s="13"/>
@@ -3505,7 +3513,7 @@
       <c r="AH143" s="12"/>
       <c r="AI143" s="12"/>
     </row>
-    <row r="144" spans="3:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:41" hidden="1" x14ac:dyDescent="0.3">
       <c r="I144" s="12"/>
       <c r="J144" s="12"/>
       <c r="L144" s="13"/>
@@ -3517,7 +3525,7 @@
       <c r="AH144" s="12"/>
       <c r="AI144" s="12"/>
     </row>
-    <row r="145" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="I145" s="12"/>
       <c r="J145" s="12"/>
       <c r="L145" s="13"/>
@@ -3529,7 +3537,8 @@
       <c r="AH145" s="12"/>
       <c r="AI145" s="12"/>
     </row>
-    <row r="146" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C146" s="13"/>
       <c r="I146" s="12"/>
       <c r="J146" s="12"/>
       <c r="L146" s="13"/>
@@ -3541,8 +3550,7 @@
       <c r="AH146" s="12"/>
       <c r="AI146" s="12"/>
     </row>
-    <row r="147" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C147" s="13"/>
+    <row r="147" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="I147" s="12"/>
       <c r="J147" s="12"/>
       <c r="L147" s="13"/>
@@ -3554,7 +3562,7 @@
       <c r="AH147" s="12"/>
       <c r="AI147" s="12"/>
     </row>
-    <row r="148" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="I148" s="12"/>
       <c r="J148" s="12"/>
       <c r="L148" s="13"/>
@@ -3566,7 +3574,7 @@
       <c r="AH148" s="12"/>
       <c r="AI148" s="12"/>
     </row>
-    <row r="149" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="I149" s="12"/>
       <c r="J149" s="12"/>
       <c r="L149" s="13"/>
@@ -3578,139 +3586,127 @@
       <c r="AH149" s="12"/>
       <c r="AI149" s="12"/>
     </row>
-    <row r="150" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I150" s="12"/>
-      <c r="J150" s="12"/>
-      <c r="L150" s="13"/>
-      <c r="M150" s="13"/>
-      <c r="Y150" s="14"/>
-      <c r="Z150" s="14"/>
+    <row r="150" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="12">
+        <f t="shared" ref="A150" si="13">A149</f>
+        <v>0</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C150" s="13">
+        <v>150</v>
+      </c>
+      <c r="D150" s="12">
+        <v>35</v>
+      </c>
+      <c r="E150" s="12">
+        <v>0</v>
+      </c>
+      <c r="F150" s="12">
+        <v>70</v>
+      </c>
+      <c r="I150" s="12">
+        <f t="shared" ref="I150" si="14">E150*D150/100</f>
+        <v>0</v>
+      </c>
+      <c r="J150" s="12">
+        <f t="shared" ref="J150" si="15">I150+J149</f>
+        <v>0</v>
+      </c>
+      <c r="L150" s="13">
+        <f t="shared" ref="L150" si="16">F150*1000/60/60</f>
+        <v>19.444444444444446</v>
+      </c>
+      <c r="M150" s="13">
+        <f t="shared" ref="M150" si="17">D150/L150</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="Y150" s="14">
+        <f t="shared" ref="Y150" si="18">L150-(M150*$AA$2)</f>
+        <v>5.7644444444444485</v>
+      </c>
+      <c r="Z150" s="14">
+        <f t="shared" ref="Z150" si="19">L150-(M150+M151)*$AA$2</f>
+        <v>5.7644444444444485</v>
+      </c>
       <c r="AF150" s="16"/>
       <c r="AG150" s="12"/>
       <c r="AH150" s="12"/>
       <c r="AI150" s="12"/>
     </row>
-    <row r="151" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="12">
-        <f t="shared" ref="A151" si="7">A150</f>
-        <v>0</v>
-      </c>
-      <c r="B151" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C151" s="13">
-        <v>150</v>
-      </c>
-      <c r="D151" s="12">
-        <v>35</v>
-      </c>
-      <c r="E151" s="12">
-        <v>0</v>
-      </c>
-      <c r="F151" s="12">
-        <v>70</v>
-      </c>
-      <c r="I151" s="12">
-        <f t="shared" ref="I151" si="8">E151*D151/100</f>
-        <v>0</v>
-      </c>
-      <c r="J151" s="12">
-        <f t="shared" ref="J151" si="9">I151+J150</f>
-        <v>0</v>
-      </c>
-      <c r="L151" s="13">
-        <f t="shared" ref="L151" si="10">F151*1000/60/60</f>
-        <v>19.444444444444446</v>
-      </c>
-      <c r="M151" s="13">
-        <f t="shared" ref="M151" si="11">D151/L151</f>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="Y151" s="14">
-        <f t="shared" ref="Y151" si="12">L151-(M151*$AA$2)</f>
-        <v>5.7644444444444485</v>
-      </c>
-      <c r="Z151" s="14">
-        <f t="shared" ref="Z151" si="13">L151-(M151+M152)*$AA$2</f>
-        <v>5.7644444444444485</v>
-      </c>
-      <c r="AF151" s="16"/>
+    <row r="151" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AF151" s="12"/>
       <c r="AG151" s="12"/>
       <c r="AH151" s="12"/>
       <c r="AI151" s="12"/>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF152" s="12"/>
       <c r="AG152" s="12"/>
       <c r="AH152" s="12"/>
       <c r="AI152" s="12"/>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF153" s="12"/>
       <c r="AG153" s="12"/>
       <c r="AH153" s="12"/>
       <c r="AI153" s="12"/>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF154" s="12"/>
       <c r="AG154" s="12"/>
       <c r="AH154" s="12"/>
       <c r="AI154" s="12"/>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF155" s="12"/>
       <c r="AG155" s="12"/>
       <c r="AH155" s="12"/>
       <c r="AI155" s="12"/>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF156" s="12"/>
       <c r="AG156" s="12"/>
       <c r="AH156" s="12"/>
       <c r="AI156" s="12"/>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF157" s="12"/>
       <c r="AG157" s="12"/>
       <c r="AH157" s="12"/>
       <c r="AI157" s="12"/>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF158" s="12"/>
       <c r="AG158" s="12"/>
       <c r="AH158" s="12"/>
       <c r="AI158" s="12"/>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF159" s="12"/>
       <c r="AG159" s="12"/>
       <c r="AH159" s="12"/>
       <c r="AI159" s="12"/>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AF160" s="12"/>
       <c r="AG160" s="12"/>
       <c r="AH160" s="12"/>
       <c r="AI160" s="12"/>
     </row>
-    <row r="161" spans="32:35" x14ac:dyDescent="0.25">
+    <row r="161" spans="32:35" x14ac:dyDescent="0.3">
       <c r="AF161" s="12"/>
       <c r="AG161" s="12"/>
       <c r="AH161" s="12"/>
       <c r="AI161" s="12"/>
     </row>
-    <row r="162" spans="32:35" x14ac:dyDescent="0.25">
+    <row r="162" spans="32:35" x14ac:dyDescent="0.3">
       <c r="AF162" s="12"/>
       <c r="AG162" s="12"/>
       <c r="AH162" s="12"/>
       <c r="AI162" s="12"/>
     </row>
-    <row r="163" spans="32:35" x14ac:dyDescent="0.25">
-      <c r="AF163" s="12"/>
-      <c r="AG163" s="12"/>
-      <c r="AH163" s="12"/>
-      <c r="AI163" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>